<commit_message>
f/mmcdaniel-baroreceptors: Tune COPD severity, update respiratory table
</commit_message>
<xml_diff>
--- a/share/doc/validation/Scenarios/RespiratoryValidation.xlsx
+++ b/share/doc/validation/Scenarios/RespiratoryValidation.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjectPrograms\BioGears\core\share\doc\validation\Scenarios\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="315" yWindow="525" windowWidth="15045" windowHeight="7620" tabRatio="643" activeTab="8"/>
+    <workbookView xWindow="312" yWindow="528" windowWidth="15048" windowHeight="7620" tabRatio="643"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="21" r:id="rId1"/>
@@ -28,12 +33,12 @@
     <definedName name="_xlnm.Print_Area" localSheetId="7">MainstemIntubation!#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Summary!$B$1:$J$17</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1877" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1877" uniqueCount="255">
   <si>
     <t>Oxygen Saturation</t>
   </si>
@@ -551,9 +556,6 @@
     <t>Increase @cite bergeronSME (case study of awake patient @cite izakson2013complete)</t>
   </si>
   <si>
-    <t>Increase @cite bergeronSME(case study of awake patient @cite izakson2013complete)</t>
-  </si>
-  <si>
     <t>Represents the partial (severity = 0.3) obstruction of airway due to  foreign body (obstructing material). Not severe enough to trigger CV responses.</t>
   </si>
   <si>
@@ -789,12 +791,24 @@
   </si>
   <si>
     <t>This represents failed  endotracheal intubation that led to esophageal intubation</t>
+  </si>
+  <si>
+    <t>Increase or no change @cite bergeronSME</t>
+  </si>
+  <si>
+    <t>Increase or no change @cite bergeronSME(case study of awake patient @cite izakson2013complete)</t>
+  </si>
+  <si>
+    <t>No change</t>
+  </si>
+  <si>
+    <t>&lt;/span&gt;|&lt;span class="succes"&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1631,6 +1645,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1678,7 +1695,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1713,7 +1730,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1927,27 +1944,27 @@
   </sheetPr>
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="57.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.5546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="2"/>
+    <col min="12" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>53</v>
       </c>
@@ -1964,25 +1981,25 @@
         <v>53</v>
       </c>
       <c r="F1" s="33" t="s">
+        <v>212</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="33" t="s">
         <v>213</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H1" s="33" t="s">
+      <c r="I1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="33" t="s">
         <v>214</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="J1" s="33" t="s">
-        <v>215</v>
-      </c>
       <c r="K1" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>53</v>
       </c>
@@ -2017,7 +2034,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>53</v>
       </c>
@@ -2028,7 +2045,7 @@
         <v>53</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>106</v>
@@ -2052,7 +2069,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>53</v>
       </c>
@@ -2063,31 +2080,31 @@
         <v>53</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>106</v>
       </c>
       <c r="F4" s="29">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>109</v>
       </c>
       <c r="H4" s="30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>110</v>
       </c>
       <c r="J4" s="31">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>53</v>
       </c>
@@ -2098,7 +2115,7 @@
         <v>53</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>106</v>
@@ -2122,7 +2139,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>53</v>
       </c>
@@ -2139,13 +2156,13 @@
         <v>106</v>
       </c>
       <c r="F6" s="29">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>109</v>
       </c>
       <c r="H6" s="30">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>110</v>
@@ -2157,7 +2174,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>53</v>
       </c>
@@ -2192,7 +2209,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>53</v>
       </c>
@@ -2203,7 +2220,7 @@
         <v>53</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>106</v>
@@ -2227,7 +2244,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>53</v>
       </c>
@@ -2238,7 +2255,7 @@
         <v>53</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>106</v>
@@ -2262,7 +2279,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>53</v>
       </c>
@@ -2273,7 +2290,7 @@
         <v>53</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>106</v>
@@ -2285,19 +2302,19 @@
         <v>109</v>
       </c>
       <c r="H10" s="30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>110</v>
       </c>
       <c r="J10" s="31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>53</v>
       </c>
@@ -2314,7 +2331,7 @@
         <v>106</v>
       </c>
       <c r="F11" s="29">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>109</v>
@@ -2326,13 +2343,13 @@
         <v>110</v>
       </c>
       <c r="J11" s="31">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>53</v>
       </c>
@@ -2349,7 +2366,7 @@
         <v>106</v>
       </c>
       <c r="F12" s="29">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>109</v>
@@ -2361,13 +2378,13 @@
         <v>110</v>
       </c>
       <c r="J12" s="31">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>53</v>
       </c>
@@ -2384,25 +2401,25 @@
         <v>106</v>
       </c>
       <c r="F13" s="29">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>109</v>
       </c>
       <c r="H13" s="30">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>110</v>
       </c>
       <c r="J13" s="31">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>53</v>
       </c>
@@ -2413,13 +2430,13 @@
         <v>53</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>106</v>
       </c>
       <c r="F14" s="29">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>109</v>
@@ -2431,13 +2448,13 @@
         <v>110</v>
       </c>
       <c r="J14" s="31">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>53</v>
       </c>
@@ -2448,54 +2465,54 @@
         <v>53</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>106</v>
       </c>
       <c r="F15" s="29">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>109</v>
       </c>
       <c r="H15" s="30">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>110</v>
       </c>
       <c r="J15" s="31">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K15" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B16" s="27" t="s">
+        <v>225</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>226</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>227</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>106</v>
       </c>
       <c r="F16" s="29">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>109</v>
       </c>
       <c r="H16" s="30">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>110</v>
@@ -2507,7 +2524,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>53</v>
       </c>
@@ -2518,13 +2535,13 @@
         <v>53</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>106</v>
       </c>
       <c r="F17" s="29">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>109</v>
@@ -2536,24 +2553,24 @@
         <v>110</v>
       </c>
       <c r="J17" s="31">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K17" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B18" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="28" t="s">
         <v>224</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="28" t="s">
-        <v>225</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>106</v>
@@ -2577,7 +2594,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>53</v>
       </c>
@@ -2586,7 +2603,7 @@
         <v>53</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>106</v>
@@ -2600,14 +2617,14 @@
       </c>
       <c r="H19" s="30">
         <f>SUM(H3:H18)</f>
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="I19" s="3" t="s">
         <v>110</v>
       </c>
       <c r="J19" s="31">
         <f>SUM(J3:J18)</f>
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="K19" s="3" t="s">
         <v>107</v>
@@ -2631,22 +2648,22 @@
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>53</v>
       </c>
@@ -2663,7 +2680,7 @@
         <v>53</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>53</v>
@@ -2681,7 +2698,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>53</v>
       </c>
@@ -2716,18 +2733,18 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>53</v>
@@ -2745,24 +2762,24 @@
         <v>106</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>230</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>231</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>53</v>
@@ -2786,18 +2803,18 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>53</v>
@@ -2815,24 +2832,24 @@
         <v>106</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B6" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>230</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>231</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>53</v>
@@ -2856,18 +2873,18 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>53</v>
@@ -2885,24 +2902,24 @@
         <v>106</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B8" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>230</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>231</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>53</v>
@@ -2938,48 +2955,48 @@
   </sheetPr>
   <dimension ref="A1:AA37"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="29" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="33.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="33.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="29.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="30.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="29.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="30.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="29.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="32.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="29.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="30.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="33.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="33.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="29.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="30.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="29.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="29.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="32.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="29.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="30.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="16384" width="9.140625" style="2"/>
+    <col min="28" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>53</v>
       </c>
@@ -2996,7 +3013,7 @@
         <v>53</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>53</v>
@@ -3062,7 +3079,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>53</v>
       </c>
@@ -3145,7 +3162,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>53</v>
       </c>
@@ -3226,7 +3243,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>53</v>
       </c>
@@ -3307,12 +3324,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>53</v>
       </c>
@@ -3329,7 +3346,7 @@
         <v>53</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>53</v>
@@ -3395,7 +3412,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>53</v>
       </c>
@@ -3478,7 +3495,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>53</v>
       </c>
@@ -3508,9 +3525,9 @@
         <v>76</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="L10" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="L10" s="9" t="s">
         <v>79</v>
       </c>
       <c r="M10" s="3" t="s">
@@ -3520,9 +3537,9 @@
         <v>80</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="P10" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="P10" s="18" t="s">
         <v>81</v>
       </c>
       <c r="Q10" s="3" t="s">
@@ -3559,7 +3576,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>53</v>
       </c>
@@ -3640,12 +3657,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>53</v>
       </c>
@@ -3662,7 +3679,7 @@
         <v>53</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>53</v>
@@ -3728,7 +3745,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>53</v>
       </c>
@@ -3811,7 +3828,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>53</v>
       </c>
@@ -3892,7 +3909,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>53</v>
       </c>
@@ -3973,58 +3990,58 @@
         <v>107</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J33" s="1"/>
     </row>
-    <row r="34" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="10:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J37" s="1"/>
     </row>
   </sheetData>
@@ -4044,46 +4061,46 @@
   </sheetPr>
   <dimension ref="A1:AA29"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="O1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="29.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="29.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="29.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="29.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="29.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="33.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="9.140625" style="2"/>
+    <col min="23" max="23" width="29.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="33.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>53</v>
       </c>
@@ -4160,13 +4177,13 @@
         <v>53</v>
       </c>
       <c r="Z2" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AA2" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>53</v>
       </c>
@@ -4249,7 +4266,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="150" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>53</v>
       </c>
@@ -4275,21 +4292,21 @@
         <v>105</v>
       </c>
       <c r="I4" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="J4" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="L4" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="N4" s="9" t="s">
+      <c r="N4" s="18" t="s">
         <v>89</v>
       </c>
       <c r="O4" s="3" t="s">
@@ -4326,22 +4343,22 @@
         <v>109</v>
       </c>
       <c r="Z4" s="18" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AA4" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:27" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="V5" s="15"/>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>57</v>
       </c>
       <c r="V6" s="16"/>
     </row>
-    <row r="7" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>53</v>
       </c>
@@ -4418,13 +4435,13 @@
         <v>53</v>
       </c>
       <c r="Z7" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AA7" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>53</v>
       </c>
@@ -4507,7 +4524,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>53</v>
       </c>
@@ -4537,15 +4554,15 @@
         <v>91</v>
       </c>
       <c r="K9" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="M9" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="L9" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="N9" s="9" t="s">
+      <c r="N9" s="18" t="s">
         <v>93</v>
       </c>
       <c r="O9" s="3" t="s">
@@ -4582,72 +4599,72 @@
         <v>109</v>
       </c>
       <c r="Z9" s="18" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AA9" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="V10" s="17"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="V11" s="16"/>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D24" s="1"/>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D25" s="1"/>
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D29" s="1"/>
     </row>
   </sheetData>
@@ -4667,46 +4684,46 @@
   </sheetPr>
   <dimension ref="A1:Y36"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I55" sqref="I55"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="30.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="30.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="29.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="29.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="29.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="29.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="29.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="29.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="9.140625" style="2"/>
+    <col min="26" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>53</v>
       </c>
@@ -4783,7 +4800,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>53</v>
       </c>
@@ -4860,7 +4877,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>53</v>
       </c>
@@ -4937,16 +4954,16 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="Q5" s="20"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B6" s="21" t="s">
         <v>33</v>
       </c>
       <c r="C6" s="21"/>
     </row>
-    <row r="7" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>53</v>
       </c>
@@ -5023,7 +5040,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>53</v>
       </c>
@@ -5100,7 +5117,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>53</v>
       </c>
@@ -5177,12 +5194,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>53</v>
       </c>
@@ -5259,7 +5276,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>53</v>
       </c>
@@ -5336,12 +5353,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="90" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>53</v>
@@ -5368,9 +5385,9 @@
         <v>90</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="L14" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="L14" s="19" t="s">
         <v>118</v>
       </c>
       <c r="M14" s="3" t="s">
@@ -5413,64 +5430,64 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H32" s="1"/>
     </row>
-    <row r="33" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H33" s="1"/>
     </row>
-    <row r="34" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H34" s="1"/>
     </row>
-    <row r="35" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H35" s="1"/>
     </row>
-    <row r="36" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H36" s="1"/>
     </row>
   </sheetData>
@@ -5487,44 +5504,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W26"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView topLeftCell="J11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.44140625" style="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.5546875" style="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" style="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.7109375" style="14" customWidth="1"/>
-    <col min="10" max="10" width="19.5703125" style="14" customWidth="1"/>
-    <col min="11" max="11" width="5.28515625" style="14" customWidth="1"/>
-    <col min="12" max="12" width="19.5703125" style="14" customWidth="1"/>
-    <col min="13" max="13" width="4.5703125" style="14" customWidth="1"/>
-    <col min="14" max="14" width="19.5703125" style="14" customWidth="1"/>
-    <col min="15" max="15" width="3.85546875" style="14" customWidth="1"/>
-    <col min="16" max="16" width="19.5703125" style="14" customWidth="1"/>
-    <col min="17" max="17" width="3.5703125" style="14" customWidth="1"/>
-    <col min="18" max="18" width="19.5703125" style="14" customWidth="1"/>
-    <col min="19" max="19" width="5.28515625" style="14" customWidth="1"/>
-    <col min="20" max="20" width="19.5703125" style="14" customWidth="1"/>
-    <col min="21" max="21" width="5.42578125" style="14" customWidth="1"/>
-    <col min="22" max="22" width="19.5703125" style="14" customWidth="1"/>
+    <col min="8" max="8" width="16.88671875" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.6640625" style="14" customWidth="1"/>
+    <col min="10" max="10" width="19.5546875" style="14" customWidth="1"/>
+    <col min="11" max="11" width="5.33203125" style="14" customWidth="1"/>
+    <col min="12" max="12" width="19.5546875" style="14" customWidth="1"/>
+    <col min="13" max="13" width="34.21875" style="14" customWidth="1"/>
+    <col min="14" max="14" width="19.5546875" style="14" customWidth="1"/>
+    <col min="15" max="15" width="28.109375" style="14" customWidth="1"/>
+    <col min="16" max="16" width="19.5546875" style="14" customWidth="1"/>
+    <col min="17" max="17" width="23.21875" style="14" customWidth="1"/>
+    <col min="18" max="18" width="19.5546875" style="14" customWidth="1"/>
+    <col min="19" max="19" width="30.33203125" style="14" customWidth="1"/>
+    <col min="20" max="20" width="19.5546875" style="14" customWidth="1"/>
+    <col min="21" max="21" width="5.44140625" style="14" customWidth="1"/>
+    <col min="22" max="22" width="19.5546875" style="14" customWidth="1"/>
     <col min="23" max="23" width="9" style="14" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="9.140625" style="14"/>
+    <col min="24" max="16384" width="9.109375" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B1" s="14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>53</v>
       </c>
@@ -5541,7 +5558,7 @@
         <v>53</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>53</v>
@@ -5595,7 +5612,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>53</v>
       </c>
@@ -5666,7 +5683,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>53</v>
       </c>
@@ -5677,7 +5694,7 @@
         <v>53</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>53</v>
@@ -5695,49 +5712,49 @@
         <v>106</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>108</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>108</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>108</v>
       </c>
       <c r="P4" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="Q4" s="3" t="s">
         <v>108</v>
       </c>
       <c r="R4" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="S4" s="3" t="s">
         <v>108</v>
       </c>
       <c r="T4" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="U4" s="3" t="s">
         <v>108</v>
       </c>
       <c r="V4" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="W4" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>53</v>
       </c>
@@ -5781,21 +5798,21 @@
         <v>131</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="P5" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="P5" s="19" t="s">
         <v>133</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="R5" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="R5" s="19" t="s">
         <v>133</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="T5" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="T5" s="19" t="s">
         <v>133</v>
       </c>
       <c r="U5" s="3" t="s">
@@ -5808,7 +5825,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>53</v>
       </c>
@@ -5852,9 +5869,9 @@
         <v>137</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="P6" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="P6" s="19" t="s">
         <v>138</v>
       </c>
       <c r="Q6" s="3" t="s">
@@ -5879,7 +5896,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>53</v>
       </c>
@@ -5950,7 +5967,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>53</v>
       </c>
@@ -5985,7 +6002,7 @@
         <v>108</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="M8" s="3" t="s">
         <v>108</v>
@@ -6021,7 +6038,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>53</v>
       </c>
@@ -6092,12 +6109,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B11" s="25" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>53</v>
       </c>
@@ -6114,7 +6131,7 @@
         <v>53</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>53</v>
@@ -6168,7 +6185,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>53</v>
       </c>
@@ -6239,7 +6256,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>53</v>
       </c>
@@ -6250,7 +6267,7 @@
         <v>53</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>53</v>
@@ -6268,49 +6285,49 @@
         <v>106</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>108</v>
       </c>
       <c r="L14" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="M14" s="3" t="s">
         <v>108</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="O14" s="3" t="s">
         <v>108</v>
       </c>
       <c r="P14" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="Q14" s="3" t="s">
         <v>108</v>
       </c>
       <c r="R14" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="S14" s="3" t="s">
         <v>108</v>
       </c>
       <c r="T14" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="U14" s="3" t="s">
         <v>108</v>
       </c>
       <c r="V14" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="W14" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>53</v>
       </c>
@@ -6354,21 +6371,21 @@
         <v>131</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="P15" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="P15" s="19" t="s">
         <v>133</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="R15" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="R15" s="19" t="s">
         <v>133</v>
       </c>
       <c r="S15" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="T15" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="T15" s="19" t="s">
         <v>133</v>
       </c>
       <c r="U15" s="3" t="s">
@@ -6381,7 +6398,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>53</v>
       </c>
@@ -6425,9 +6442,9 @@
         <v>151</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="P16" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="P16" s="19" t="s">
         <v>152</v>
       </c>
       <c r="Q16" s="3" t="s">
@@ -6452,7 +6469,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>53</v>
       </c>
@@ -6523,7 +6540,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>53</v>
       </c>
@@ -6594,18 +6611,18 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" s="21"/>
       <c r="C19" s="21"/>
       <c r="E19" s="21"/>
       <c r="G19" s="21"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B20" s="25" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>53</v>
       </c>
@@ -6622,7 +6639,7 @@
         <v>53</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>53</v>
@@ -6676,7 +6693,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>53</v>
       </c>
@@ -6747,7 +6764,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>53</v>
       </c>
@@ -6785,15 +6802,15 @@
         <v>136</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="N23" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="N23" s="19" t="s">
         <v>151</v>
       </c>
       <c r="O23" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="P23" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="P23" s="19" t="s">
         <v>152</v>
       </c>
       <c r="Q23" s="3" t="s">
@@ -6818,7 +6835,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>53</v>
       </c>
@@ -6853,12 +6870,12 @@
         <v>108</v>
       </c>
       <c r="L24" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="N24" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="N24" s="18" t="s">
         <v>145</v>
       </c>
       <c r="O24" s="3" t="s">
@@ -6889,7 +6906,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>53</v>
       </c>
@@ -6960,7 +6977,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>53</v>
       </c>
@@ -7045,34 +7062,34 @@
   <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I17" sqref="I16:I17"/>
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2" style="14" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.44140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9" style="14" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="2"/>
+    <col min="20" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>53</v>
       </c>
@@ -7089,7 +7106,7 @@
         <v>53</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>53</v>
@@ -7131,7 +7148,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>53</v>
       </c>
@@ -7190,7 +7207,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="105" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>53</v>
       </c>
@@ -7201,7 +7218,7 @@
         <v>53</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>53</v>
@@ -7225,13 +7242,13 @@
         <v>108</v>
       </c>
       <c r="L3" s="23" t="s">
-        <v>122</v>
+        <v>251</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="N3" s="24" t="s">
-        <v>172</v>
+        <v>108</v>
+      </c>
+      <c r="N3" s="23" t="s">
+        <v>252</v>
       </c>
       <c r="O3" s="3" t="s">
         <v>108</v>
@@ -7249,7 +7266,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>53</v>
       </c>
@@ -7278,37 +7295,37 @@
         <v>106</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>108</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>108</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>108</v>
       </c>
       <c r="P4" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="Q4" s="3" t="s">
         <v>108</v>
       </c>
       <c r="R4" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="S4" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>53</v>
       </c>
@@ -7319,7 +7336,7 @@
         <v>53</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>53</v>
@@ -7346,9 +7363,9 @@
         <v>122</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="N5" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="N5" s="23" t="s">
         <v>170</v>
       </c>
       <c r="O5" s="3" t="s">
@@ -7367,7 +7384,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>53</v>
       </c>
@@ -7396,37 +7413,37 @@
         <v>106</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>108</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>108</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="O6" s="3" t="s">
         <v>108</v>
       </c>
       <c r="P6" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="Q6" s="3" t="s">
         <v>108</v>
       </c>
       <c r="R6" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="S6" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>53</v>
       </c>
@@ -7437,7 +7454,7 @@
         <v>53</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>53</v>
@@ -7464,9 +7481,9 @@
         <v>122</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="N7" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="N7" s="23" t="s">
         <v>170</v>
       </c>
       <c r="O7" s="3" t="s">
@@ -7485,7 +7502,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>53</v>
       </c>
@@ -7514,31 +7531,31 @@
         <v>106</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>108</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="M8" s="3" t="s">
         <v>108</v>
       </c>
       <c r="N8" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="O8" s="3" t="s">
         <v>108</v>
       </c>
       <c r="P8" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="Q8" s="3" t="s">
         <v>108</v>
       </c>
       <c r="R8" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="S8" s="3" t="s">
         <v>107</v>
@@ -7561,35 +7578,35 @@
   </sheetPr>
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2" style="14" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2" style="14" customWidth="1"/>
     <col min="4" max="4" width="26" style="2" customWidth="1"/>
     <col min="5" max="5" width="2" style="14" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2" style="14" customWidth="1"/>
     <col min="8" max="8" width="22" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.44140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9" style="14" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="2"/>
+    <col min="20" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>53</v>
       </c>
@@ -7606,13 +7623,13 @@
         <v>53</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>53</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>53</v>
@@ -7648,7 +7665,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>53</v>
       </c>
@@ -7707,7 +7724,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>53</v>
       </c>
@@ -7718,7 +7735,7 @@
         <v>53</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>53</v>
@@ -7733,40 +7750,40 @@
         <v>180</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J3" s="26" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="L3" s="26" t="s">
-        <v>186</v>
+        <v>108</v>
+      </c>
+      <c r="L3" s="23" t="s">
+        <v>253</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="N3" s="26" t="s">
-        <v>185</v>
+        <v>108</v>
+      </c>
+      <c r="N3" s="23" t="s">
+        <v>253</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="P3" s="26" t="s">
-        <v>185</v>
+        <v>108</v>
+      </c>
+      <c r="P3" s="23" t="s">
+        <v>253</v>
       </c>
       <c r="Q3" s="3" t="s">
         <v>108</v>
       </c>
       <c r="R3" s="23" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="S3" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>53</v>
       </c>
@@ -7795,48 +7812,48 @@
         <v>106</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>108</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>108</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>108</v>
       </c>
       <c r="P4" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="Q4" s="3" t="s">
         <v>108</v>
       </c>
       <c r="R4" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="S4" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>53</v>
@@ -7860,31 +7877,31 @@
         <v>108</v>
       </c>
       <c r="L5" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="N5" s="23" t="s">
-        <v>185</v>
+        <v>110</v>
+      </c>
+      <c r="N5" s="24" t="s">
+        <v>184</v>
       </c>
       <c r="O5" s="3" t="s">
         <v>110</v>
       </c>
       <c r="P5" s="24" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="Q5" s="3" t="s">
         <v>108</v>
       </c>
       <c r="R5" s="23" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="S5" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>53</v>
       </c>
@@ -7913,48 +7930,48 @@
         <v>106</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>108</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>108</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="O6" s="3" t="s">
         <v>108</v>
       </c>
       <c r="P6" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="Q6" s="3" t="s">
         <v>108</v>
       </c>
       <c r="R6" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="S6" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="72" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>53</v>
@@ -7978,31 +7995,31 @@
         <v>108</v>
       </c>
       <c r="L7" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="N7" s="23" t="s">
-        <v>185</v>
+        <v>110</v>
+      </c>
+      <c r="N7" s="24" t="s">
+        <v>184</v>
       </c>
       <c r="O7" s="3" t="s">
         <v>110</v>
       </c>
       <c r="P7" s="24" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="Q7" s="3" t="s">
         <v>108</v>
       </c>
       <c r="R7" s="23" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="S7" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>53</v>
       </c>
@@ -8031,31 +8048,31 @@
         <v>106</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>108</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="M8" s="3" t="s">
         <v>108</v>
       </c>
       <c r="N8" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="O8" s="3" t="s">
         <v>108</v>
       </c>
       <c r="P8" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="Q8" s="3" t="s">
         <v>108</v>
       </c>
       <c r="R8" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="S8" s="3" t="s">
         <v>107</v>
@@ -8079,37 +8096,37 @@
   <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2" style="14" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="2" style="14" customWidth="1"/>
-    <col min="4" max="4" width="30.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2" style="14" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2" style="14" customWidth="1"/>
     <col min="8" max="8" width="22" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.44140625" style="14" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9" style="14" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="20" style="2" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" style="2"/>
+    <col min="21" max="21" width="9.109375" style="2"/>
     <col min="22" max="22" width="13" style="2" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="2"/>
+    <col min="23" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>53</v>
       </c>
@@ -8126,13 +8143,13 @@
         <v>53</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>53</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>53</v>
@@ -8168,7 +8185,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>53</v>
       </c>
@@ -8227,18 +8244,18 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>53</v>
@@ -8256,37 +8273,37 @@
         <v>106</v>
       </c>
       <c r="J3" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="L3" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="K3" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="L3" s="26" t="s">
+      <c r="M3" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="N3" s="23" t="s">
         <v>191</v>
       </c>
-      <c r="M3" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="N3" s="26" t="s">
+      <c r="O3" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="P3" s="23" t="s">
         <v>192</v>
       </c>
-      <c r="O3" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="P3" s="26" t="s">
-        <v>193</v>
-      </c>
       <c r="Q3" s="3" t="s">
         <v>108</v>
       </c>
       <c r="R3" s="23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="S3" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>53</v>
       </c>
@@ -8297,7 +8314,7 @@
         <v>53</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>53</v>
@@ -8315,37 +8332,37 @@
         <v>106</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>108</v>
       </c>
       <c r="L4" s="23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>108</v>
       </c>
       <c r="N4" s="23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>108</v>
       </c>
       <c r="P4" s="23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q4" s="3" t="s">
         <v>108</v>
       </c>
       <c r="R4" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="S4" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>53</v>
       </c>
@@ -8356,7 +8373,7 @@
         <v>53</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>53</v>
@@ -8374,48 +8391,48 @@
         <v>106</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>108</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="M5" s="3" t="s">
         <v>108</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O5" s="3" t="s">
         <v>108</v>
       </c>
       <c r="P5" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="Q5" s="3" t="s">
         <v>108</v>
       </c>
       <c r="R5" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="S5" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>53</v>
@@ -8433,37 +8450,37 @@
         <v>106</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>108</v>
       </c>
       <c r="L6" s="23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>108</v>
       </c>
       <c r="N6" s="23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O6" s="3" t="s">
         <v>108</v>
       </c>
       <c r="P6" s="23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q6" s="3" t="s">
         <v>108</v>
       </c>
       <c r="R6" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="S6" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>53</v>
       </c>
@@ -8474,7 +8491,7 @@
         <v>53</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>53</v>
@@ -8492,31 +8509,31 @@
         <v>106</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>108</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="M7" s="3" t="s">
         <v>108</v>
       </c>
       <c r="N7" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O7" s="3" t="s">
         <v>108</v>
       </c>
       <c r="P7" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="Q7" s="3" t="s">
         <v>108</v>
       </c>
       <c r="R7" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="S7" s="3" t="s">
         <v>107</v>
@@ -8539,35 +8556,35 @@
   </sheetPr>
   <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2" style="14" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2" style="14" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2" style="14" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2" style="14" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.44140625" style="14" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9" style="14" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="2"/>
+    <col min="20" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>53</v>
       </c>
@@ -8584,49 +8601,49 @@
         <v>53</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>53</v>
       </c>
       <c r="H1" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" s="22" t="s">
         <v>197</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="L1" s="22" t="s">
+      <c r="M1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="M1" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="P1" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="O1" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="R1" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="Q1" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>201</v>
-      </c>
       <c r="S1" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>53</v>
       </c>
@@ -8685,12 +8702,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>53</v>
@@ -8708,43 +8725,43 @@
         <v>53</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>106</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="L3" s="24" t="s">
-        <v>202</v>
+        <v>108</v>
+      </c>
+      <c r="L3" s="23" t="s">
+        <v>201</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="N3" s="24" t="s">
-        <v>202</v>
+        <v>254</v>
+      </c>
+      <c r="N3" s="23" t="s">
+        <v>201</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="P3" s="24" t="s">
-        <v>202</v>
+        <v>108</v>
+      </c>
+      <c r="P3" s="23" t="s">
+        <v>201</v>
       </c>
       <c r="Q3" s="3" t="s">
         <v>108</v>
       </c>
       <c r="R3" s="23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="S3" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>53</v>
       </c>
@@ -8755,7 +8772,7 @@
         <v>53</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>53</v>
@@ -8773,37 +8790,37 @@
         <v>106</v>
       </c>
       <c r="J4" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="L4" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="N4" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="P4" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="R4" s="9" t="s">
         <v>219</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="L4" s="23" t="s">
-        <v>203</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="N4" s="23" t="s">
-        <v>203</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="P4" s="23" t="s">
-        <v>203</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="R4" s="9" t="s">
-        <v>220</v>
       </c>
       <c r="S4" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>53</v>
       </c>
@@ -8832,31 +8849,31 @@
         <v>106</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>108</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="M5" s="3" t="s">
         <v>108</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="O5" s="3" t="s">
         <v>108</v>
       </c>
       <c r="P5" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="Q5" s="3" t="s">
         <v>108</v>
       </c>
       <c r="R5" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="S5" s="3" t="s">
         <v>107</v>

</xml_diff>

<commit_message>
f/mmcdaniel-baroreceptors: CDM additions and documentation update
Missed xsd file in last commit for mean pleural pressure

Update respiratory documentation for pneumothorax and asthma.
</commit_message>
<xml_diff>
--- a/share/doc/validation/Scenarios/RespiratoryValidation.xlsx
+++ b/share/doc/validation/Scenarios/RespiratoryValidation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="312" yWindow="528" windowWidth="15048" windowHeight="7620" tabRatio="643"/>
+    <workbookView xWindow="312" yWindow="528" windowWidth="15048" windowHeight="7620" tabRatio="643" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="21" r:id="rId1"/>
@@ -1944,8 +1944,8 @@
   </sheetPr>
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2086,7 +2086,7 @@
         <v>106</v>
       </c>
       <c r="F4" s="29">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>109</v>
@@ -2098,7 +2098,7 @@
         <v>110</v>
       </c>
       <c r="J4" s="31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>107</v>
@@ -2127,13 +2127,13 @@
         <v>109</v>
       </c>
       <c r="H5" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>110</v>
       </c>
       <c r="J5" s="31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>107</v>
@@ -2331,7 +2331,7 @@
         <v>106</v>
       </c>
       <c r="F11" s="29">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>109</v>
@@ -2343,7 +2343,7 @@
         <v>110</v>
       </c>
       <c r="J11" s="31">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>107</v>
@@ -2366,7 +2366,7 @@
         <v>106</v>
       </c>
       <c r="F12" s="29">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>109</v>
@@ -2378,7 +2378,7 @@
         <v>110</v>
       </c>
       <c r="J12" s="31">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>107</v>
@@ -2401,19 +2401,19 @@
         <v>106</v>
       </c>
       <c r="F13" s="29">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>109</v>
       </c>
       <c r="H13" s="30">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>110</v>
       </c>
       <c r="J13" s="31">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>107</v>
@@ -2610,21 +2610,21 @@
       </c>
       <c r="F19" s="29">
         <f>SUM(F3:F18)</f>
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>109</v>
       </c>
       <c r="H19" s="30">
         <f>SUM(H3:H18)</f>
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I19" s="3" t="s">
         <v>110</v>
       </c>
       <c r="J19" s="31">
         <f>SUM(J3:J18)</f>
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="K19" s="3" t="s">
         <v>107</v>
@@ -2955,8 +2955,8 @@
   </sheetPr>
   <dimension ref="A1:AA37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView topLeftCell="P1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:AA17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3537,15 +3537,15 @@
         <v>80</v>
       </c>
       <c r="O10" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="P10" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q10" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="P10" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q10" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="R10" s="12" t="s">
+      <c r="R10" s="18" t="s">
         <v>72</v>
       </c>
       <c r="S10" s="3" t="s">
@@ -3876,9 +3876,9 @@
         <v>85</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="R16" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="R16" s="18" t="s">
         <v>74</v>
       </c>
       <c r="S16" s="3" t="s">
@@ -5504,8 +5504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W26"/>
   <sheetViews>
-    <sheetView topLeftCell="J11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+    <sheetView tabSelected="1" topLeftCell="I11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="X20" sqref="X20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5798,9 +5798,9 @@
         <v>131</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="P5" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="P5" s="9" t="s">
         <v>133</v>
       </c>
       <c r="Q5" s="3" t="s">
@@ -5810,9 +5810,9 @@
         <v>133</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="T5" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="T5" s="9" t="s">
         <v>133</v>
       </c>
       <c r="U5" s="3" t="s">
@@ -5869,9 +5869,9 @@
         <v>137</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="P6" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="P6" s="9" t="s">
         <v>138</v>
       </c>
       <c r="Q6" s="3" t="s">
@@ -5881,9 +5881,9 @@
         <v>138</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="T6" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="T6" s="9" t="s">
         <v>138</v>
       </c>
       <c r="U6" s="3" t="s">
@@ -5940,9 +5940,9 @@
         <v>141</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="P7" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="P7" s="18" t="s">
         <v>142</v>
       </c>
       <c r="Q7" s="3" t="s">
@@ -5952,9 +5952,9 @@
         <v>142</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="T7" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="T7" s="18" t="s">
         <v>142</v>
       </c>
       <c r="U7" s="3" t="s">
@@ -6082,9 +6082,9 @@
         <v>148</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="P9" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="P9" s="9" t="s">
         <v>149</v>
       </c>
       <c r="Q9" s="3" t="s">
@@ -6094,9 +6094,9 @@
         <v>149</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="T9" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="T9" s="9" t="s">
         <v>149</v>
       </c>
       <c r="U9" s="3" t="s">
@@ -6371,9 +6371,9 @@
         <v>131</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="P15" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="P15" s="9" t="s">
         <v>133</v>
       </c>
       <c r="Q15" s="3" t="s">
@@ -6383,9 +6383,9 @@
         <v>133</v>
       </c>
       <c r="S15" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="T15" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="T15" s="9" t="s">
         <v>133</v>
       </c>
       <c r="U15" s="3" t="s">
@@ -6442,9 +6442,9 @@
         <v>151</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="P16" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="P16" s="9" t="s">
         <v>152</v>
       </c>
       <c r="Q16" s="3" t="s">
@@ -6454,9 +6454,9 @@
         <v>138</v>
       </c>
       <c r="S16" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="T16" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="T16" s="9" t="s">
         <v>138</v>
       </c>
       <c r="U16" s="3" t="s">
@@ -6513,9 +6513,9 @@
         <v>153</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="P17" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="P17" s="18" t="s">
         <v>154</v>
       </c>
       <c r="Q17" s="3" t="s">
@@ -6525,9 +6525,9 @@
         <v>154</v>
       </c>
       <c r="S17" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="T17" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="T17" s="18" t="s">
         <v>154</v>
       </c>
       <c r="U17" s="3" t="s">
@@ -6584,9 +6584,9 @@
         <v>157</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="P18" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="P18" s="9" t="s">
         <v>149</v>
       </c>
       <c r="Q18" s="3" t="s">
@@ -6596,9 +6596,9 @@
         <v>149</v>
       </c>
       <c r="S18" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="T18" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="T18" s="9" t="s">
         <v>149</v>
       </c>
       <c r="U18" s="3" t="s">
@@ -6802,15 +6802,15 @@
         <v>136</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="N23" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="N23" s="9" t="s">
         <v>151</v>
       </c>
       <c r="O23" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="P23" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="P23" s="9" t="s">
         <v>152</v>
       </c>
       <c r="Q23" s="3" t="s">
@@ -6820,9 +6820,9 @@
         <v>152</v>
       </c>
       <c r="S23" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="T23" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="T23" s="9" t="s">
         <v>152</v>
       </c>
       <c r="U23" s="3" t="s">
@@ -6950,9 +6950,9 @@
         <v>148</v>
       </c>
       <c r="O25" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="P25" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="P25" s="9" t="s">
         <v>159</v>
       </c>
       <c r="Q25" s="3" t="s">
@@ -6962,9 +6962,9 @@
         <v>159</v>
       </c>
       <c r="S25" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="T25" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="T25" s="9" t="s">
         <v>159</v>
       </c>
       <c r="U25" s="3" t="s">
@@ -7021,9 +7021,9 @@
         <v>157</v>
       </c>
       <c r="O26" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="P26" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="P26" s="9" t="s">
         <v>149</v>
       </c>
       <c r="Q26" s="3" t="s">
@@ -7033,9 +7033,9 @@
         <v>149</v>
       </c>
       <c r="S26" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="T26" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="T26" s="9" t="s">
         <v>149</v>
       </c>
       <c r="U26" s="3" t="s">

</xml_diff>